<commit_message>
Added proper colors based on availability
</commit_message>
<xml_diff>
--- a/grouping_results_report.xlsx
+++ b/grouping_results_report.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="121">
   <si>
     <t>Student Id</t>
   </si>
@@ -122,7 +122,7 @@
     <t>Score</t>
   </si>
   <si>
-    <t>jsmith1;jdoe2;mmuster3;jschmo4</t>
+    <t>jsmith1;mmuster3;jschmo4;jdoe2</t>
   </si>
   <si>
     <t>jdoe2/mmuster3;jdoe2/jschmo4;jsmith1/jdoe2;mmuster3/jsmith1</t>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>target_minus_one_allowed</t>
+  </si>
+  <si>
+    <t>no_survey_group_method</t>
   </si>
   <si>
     <t>grouping_passes</t>
@@ -776,7 +779,7 @@
       <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F2" t="s">
@@ -817,7 +820,7 @@
       <c r="D3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F3" t="s">
@@ -852,7 +855,7 @@
       <c r="C4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F4" t="s">
@@ -887,7 +890,7 @@
       <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F5" t="s">
@@ -1070,13 +1073,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -1131,10 +1134,13 @@
       <c r="R1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:18">
+      <c r="S1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -1146,10 +1152,10 @@
         <v>0</v>
       </c>
       <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
         <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>62</v>
       </c>
       <c r="G2" t="s">
         <v>63</v>
@@ -1166,8 +1172,8 @@
       <c r="K2" t="s">
         <v>67</v>
       </c>
-      <c r="L2" t="b">
-        <v>1</v>
+      <c r="L2" t="s">
+        <v>68</v>
       </c>
       <c r="M2" t="b">
         <v>1</v>
@@ -1179,66 +1185,69 @@
         <v>1</v>
       </c>
       <c r="P2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="b">
         <v>0</v>
       </c>
-      <c r="Q2" t="b">
-        <v>1</v>
-      </c>
       <c r="R2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:18">
-      <c r="I3" t="s">
-        <v>68</v>
-      </c>
+      <c r="S2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="J3" t="s">
         <v>69</v>
       </c>
       <c r="K3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="I4" t="s">
+      <c r="L3" t="s">
         <v>71</v>
       </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="J4" t="s">
         <v>72</v>
       </c>
       <c r="K4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="5" spans="1:18">
-      <c r="I5" t="s">
+      <c r="L4" t="s">
         <v>74</v>
       </c>
-      <c r="K5" t="s">
+    </row>
+    <row r="5" spans="1:19">
+      <c r="J5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="6" spans="1:18">
-      <c r="I6" t="s">
+      <c r="L5" t="s">
         <v>76</v>
       </c>
-      <c r="K6" t="s">
+    </row>
+    <row r="6" spans="1:19">
+      <c r="J6" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="K7" t="s">
+      <c r="L6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
-      <c r="K8" t="s">
+    <row r="7" spans="1:19">
+      <c r="L7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
-      <c r="K9" t="s">
+    <row r="8" spans="1:19">
+      <c r="L8" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="L9" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1256,214 +1265,214 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" t="s">
         <v>81</v>
       </c>
-      <c r="B1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="O1" t="s">
+        <v>86</v>
+      </c>
+      <c r="P1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R1" t="s">
+        <v>69</v>
+      </c>
+      <c r="S1" t="s">
+        <v>72</v>
+      </c>
+      <c r="T1" t="s">
+        <v>75</v>
+      </c>
+      <c r="U1" t="s">
+        <v>77</v>
+      </c>
+      <c r="V1" t="s">
         <v>67</v>
       </c>
-      <c r="H1" t="s">
+      <c r="W1" t="s">
         <v>70</v>
       </c>
-      <c r="I1" t="s">
+      <c r="X1" t="s">
         <v>73</v>
-      </c>
-      <c r="J1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K1" t="s">
-        <v>77</v>
-      </c>
-      <c r="L1" t="s">
-        <v>78</v>
-      </c>
-      <c r="M1" t="s">
-        <v>79</v>
-      </c>
-      <c r="N1" t="s">
-        <v>80</v>
-      </c>
-      <c r="O1" t="s">
-        <v>85</v>
-      </c>
-      <c r="P1" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>65</v>
-      </c>
-      <c r="R1" t="s">
-        <v>68</v>
-      </c>
-      <c r="S1" t="s">
-        <v>71</v>
-      </c>
-      <c r="T1" t="s">
-        <v>74</v>
-      </c>
-      <c r="U1" t="s">
-        <v>76</v>
-      </c>
-      <c r="V1" t="s">
-        <v>66</v>
-      </c>
-      <c r="W1" t="s">
-        <v>69</v>
-      </c>
-      <c r="X1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:24">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="Q2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="V2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="W2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:24">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="L3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="O3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="P3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="Q3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="R3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="V3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="W3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:24">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C4" t="s">
         <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="M4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="O4" t="s">
+        <v>109</v>
+      </c>
+      <c r="P4" t="s">
         <v>108</v>
       </c>
-      <c r="P4" t="s">
-        <v>107</v>
-      </c>
       <c r="Q4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="R4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="V4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:24">
@@ -1471,21 +1480,21 @@
         <v>24</v>
       </c>
       <c r="H5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:24">
       <c r="C6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>